<commit_message>
Add more articles and photos
</commit_message>
<xml_diff>
--- a/docs/xlcdapp_article_list.xlsx
+++ b/docs/xlcdapp_article_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\git\chiachang100\xlcdapp\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B936D812-73A7-4058-8648-761723A497A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D531388-7475-44EB-AC68-F9369D533A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="1350" windowWidth="19770" windowHeight="11993" xr2:uid="{A932B94A-463B-433C-A50E-1D8D05A6193F}"/>
+    <workbookView xWindow="570" yWindow="1620" windowWidth="19770" windowHeight="11993" xr2:uid="{A932B94A-463B-433C-A50E-1D8D05A6193F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="114">
   <si>
     <t>id</t>
   </si>
@@ -289,6 +289,84 @@
   </si>
   <si>
     <t>沒有救自己的耶穌 | 曾興才牧師 | 20220410</t>
+  </si>
+  <si>
+    <t>以弗所書 5:1</t>
+  </si>
+  <si>
+    <t>xlcdapp_photo_15</t>
+  </si>
+  <si>
+    <t>夏</t>
+  </si>
+  <si>
+    <t>上帝榮耀的豐富</t>
+  </si>
+  <si>
+    <t>腓立比書 4:19</t>
+  </si>
+  <si>
+    <t>AGTacXFkFDQ</t>
+  </si>
+  <si>
+    <t>耶穌必能為你平靜風浪 | 曾興才牧師 | 20200315</t>
+  </si>
+  <si>
+    <t>xlcdapp_photo_16</t>
+  </si>
+  <si>
+    <t>xlcdapp_photo_17</t>
+  </si>
+  <si>
+    <t>xlcdapp_photo_18</t>
+  </si>
+  <si>
+    <t>xlcdapp_photo_19</t>
+  </si>
+  <si>
+    <t>xlcdapp_photo_20</t>
+  </si>
+  <si>
+    <t>起初的愛心</t>
+  </si>
+  <si>
+    <t>要像小孩子</t>
+  </si>
+  <si>
+    <t>應當一無掛慮</t>
+  </si>
+  <si>
+    <t>不要以惡報惡</t>
+  </si>
+  <si>
+    <t>要孝敬父母</t>
+  </si>
+  <si>
+    <t>啟示錄 2:4</t>
+  </si>
+  <si>
+    <t>馬可福音 10:15</t>
+  </si>
+  <si>
+    <t>jNSw1OJkzdY</t>
+  </si>
+  <si>
+    <t>經歷感恩的能力 | 曾興才牧師 | 20221113</t>
+  </si>
+  <si>
+    <t>hbxbb2vvbcw</t>
+  </si>
+  <si>
+    <t>耶穌降⽣的三⼤恢復 | 曾興才牧師 | 20221211</t>
+  </si>
+  <si>
+    <t>腓立比書 4:6</t>
+  </si>
+  <si>
+    <t>PWT_rjy2jbM</t>
+  </si>
+  <si>
+    <t>神的殿，我們的家 | 曾興才牧師 | 20220814</t>
   </si>
 </sst>
 </file>
@@ -366,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -381,10 +459,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -397,9 +471,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -715,10 +786,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACDC77D5-3670-42B0-B2C8-F3E5E18EC549}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -747,38 +818,38 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
     </row>
-    <row r="3" spans="1:11" s="12" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
-      <c r="A3" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="11" t="s">
+    <row r="3" spans="1:11" s="10" customFormat="1" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="A3" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="G3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="J3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="K3" s="11" t="s">
+      <c r="K3" s="9" t="s">
         <v>13</v>
       </c>
     </row>
@@ -866,7 +937,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="1">
-        <f t="shared" ref="B7:B17" si="0">B6+1</f>
+        <f t="shared" ref="B7:B24" si="0">B6+1</f>
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -1257,87 +1328,296 @@
         <v>14</v>
       </c>
     </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A18" s="1">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F18" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" t="s">
+        <v>87</v>
+      </c>
+      <c r="H18" s="1">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1">
+        <v>1</v>
+      </c>
+      <c r="J18" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>0</v>
       </c>
       <c r="B19" s="1">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" t="s">
+        <v>93</v>
+      </c>
+      <c r="G19" t="s">
+        <v>94</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1</v>
+      </c>
+      <c r="J19" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A20" s="1">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E20" t="s">
+        <v>95</v>
+      </c>
+      <c r="F20" t="s">
+        <v>107</v>
+      </c>
+      <c r="G20" t="s">
+        <v>108</v>
+      </c>
+      <c r="H20" s="1">
+        <v>1</v>
+      </c>
+      <c r="I20" s="1">
+        <v>1</v>
+      </c>
+      <c r="J20" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A21" s="1">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" t="s">
+        <v>96</v>
+      </c>
+      <c r="F21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" t="s">
+        <v>110</v>
+      </c>
+      <c r="H21" s="1">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1">
+        <v>1</v>
+      </c>
+      <c r="J21" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A22" s="1">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" t="s">
+        <v>112</v>
+      </c>
+      <c r="G22" t="s">
+        <v>113</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+      <c r="J22" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A23" s="1">
+        <v>0</v>
+      </c>
+      <c r="B23" s="1">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E23" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A24" s="1">
+        <v>0</v>
+      </c>
+      <c r="B24" s="1">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A26" s="1">
+        <v>0</v>
+      </c>
+      <c r="B26" s="1">
         <v>52</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C26" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E26" t="s">
         <v>81</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F26" t="s">
         <v>80</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G26" t="s">
         <v>82</v>
       </c>
-      <c r="H19" s="1">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1">
-        <v>1</v>
-      </c>
-      <c r="J19" s="1" t="b">
-        <v>1</v>
-      </c>
-      <c r="K19" s="1" t="s">
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>1</v>
+      </c>
+      <c r="J26" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-    </row>
-    <row r="23" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="6">
-        <v>0</v>
-      </c>
-      <c r="B23" s="6">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A29" s="6"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A30" s="1">
+        <v>0</v>
+      </c>
+      <c r="B30" s="1">
         <f>B17+1</f>
         <v>14</v>
       </c>
-      <c r="C23" s="13" t="s">
+      <c r="C30" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D23" s="13" t="s">
+      <c r="D30" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E30" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="7" t="s">
+      <c r="F30" t="s">
         <v>86</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G30" t="s">
         <v>87</v>
       </c>
-      <c r="H23" s="6">
-        <v>0</v>
-      </c>
-      <c r="I23" s="6">
-        <v>1</v>
-      </c>
-      <c r="J23" s="6" t="b">
-        <v>1</v>
-      </c>
-      <c r="K23" s="6"/>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1" t="b">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>